<commit_message>
adding the expense section where i show all the expense in the form of Line Chart
</commit_message>
<xml_diff>
--- a/backend/income_details.xlsx
+++ b/backend/income_details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,16 +415,63 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="str">
+        <v>salary</v>
+      </c>
       <c r="B2">
-        <v>3000</v>
+        <v>12500</v>
       </c>
       <c r="C2" s="1">
-        <v>45798.52537037037</v>
+        <v>45809.22928240741</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Trading</v>
+      </c>
+      <c r="B3">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45809.22928240741</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Youtube Revenue</v>
+      </c>
+      <c r="B4">
+        <v>9500</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45809.22928240741</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Interest From Saving account</v>
+      </c>
+      <c r="B5">
+        <v>4300</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45806.22928240741</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="B6">
+        <v>5600</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45797.92650462963</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>